<commit_message>
thay doi lan dau
</commit_message>
<xml_diff>
--- a/myfile.xlsx
+++ b/myfile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\myfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>MY FILE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sua dipoi lanmne </t>
   </si>
 </sst>
 </file>
@@ -42,12 +45,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -62,8 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -344,18 +354,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2"/>
+  <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
thay doi lan 3
</commit_message>
<xml_diff>
--- a/myfile.xlsx
+++ b/myfile.xlsx
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>MY FILE</t>
   </si>
   <si>
     <t xml:space="preserve">sua dipoi lanmne </t>
+  </si>
+  <si>
+    <t xml:space="preserve">thay doi lan 2 </t>
   </si>
 </sst>
 </file>
@@ -354,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E5"/>
+  <dimension ref="B2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,6 +376,16 @@
       </c>
       <c r="E5" s="1"/>
     </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
thay doi lan cuoi
</commit_message>
<xml_diff>
--- a/myfile.xlsx
+++ b/myfile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>MY FILE</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t xml:space="preserve">thay doi lan 2 </t>
+  </si>
+  <si>
+    <t>thay doi lan 3</t>
   </si>
 </sst>
 </file>
@@ -357,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E8"/>
+  <dimension ref="B2:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,6 +389,11 @@
         <v>111</v>
       </c>
     </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>